<commit_message>
Completed more 10K Steps trials
</commit_message>
<xml_diff>
--- a/model_testing/shortjokesclean/shortjokesclean.xlsx
+++ b/model_testing/shortjokesclean/shortjokesclean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malik Shalash\Documents\Development\School\CECS-696\gpt-2-joker-bot\model_testing\shortjokesclean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACFCDAA-BF8F-4148-9C4C-C5DDE0A10D48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7DD1C6-ADBF-41BA-AB61-5BF404B3C0BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>Batch Size</t>
   </si>
@@ -97,6 +97,30 @@
   </si>
   <si>
     <t>(LR = 10000)</t>
+  </si>
+  <si>
+    <t>Loss 1</t>
+  </si>
+  <si>
+    <t>Loss 2</t>
+  </si>
+  <si>
+    <t>Loss 3</t>
+  </si>
+  <si>
+    <t>Loss 4</t>
+  </si>
+  <si>
+    <t>Loss 5</t>
+  </si>
+  <si>
+    <t>Loss 6</t>
+  </si>
+  <si>
+    <t>Loss 7</t>
+  </si>
+  <si>
+    <t>Loss 8</t>
   </si>
 </sst>
 </file>
@@ -151,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -303,6 +327,72 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -312,7 +402,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -335,6 +425,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -618,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,14 +920,18 @@
       <c r="B20" s="6">
         <v>1</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="E20" s="21">
+        <v>3068.42</v>
+      </c>
+      <c r="F20" s="18">
+        <v>3052.0412999999999</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -839,14 +940,18 @@
       <c r="B21" s="7">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="D21" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>7239.3440000000001</v>
+      </c>
+      <c r="F21" s="19">
+        <v>7240.6790000000001</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -855,14 +960,18 @@
       <c r="B22" s="6">
         <v>5000</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
+      <c r="D22" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>6803.4939999999997</v>
+      </c>
+      <c r="F22" s="19">
+        <v>6808.009</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -871,6 +980,18 @@
       <c r="B23" s="6">
         <v>10000</v>
       </c>
+      <c r="D23" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>6201.4008000000003</v>
+      </c>
+      <c r="F23" s="19">
+        <v>6191.0739999999996</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -879,6 +1000,18 @@
       <c r="B24" s="6">
         <v>400</v>
       </c>
+      <c r="D24" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>6005.973</v>
+      </c>
+      <c r="F24" s="19">
+        <v>5998.9139999999998</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -887,6 +1020,18 @@
       <c r="B25" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="D25" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>5897.692</v>
+      </c>
+      <c r="F25" s="19">
+        <v>5897.4059999999999</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -895,6 +1040,18 @@
       <c r="B26" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="D26" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26">
+        <v>5821.1379999999999</v>
+      </c>
+      <c r="F26" s="19">
+        <v>5826.5320000000002</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -903,6 +1060,56 @@
       <c r="B27" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="D27" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27">
+        <v>5769.4511000000002</v>
+      </c>
+      <c r="F27" s="19">
+        <v>5770.317</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28">
+        <v>5721.3071</v>
+      </c>
+      <c r="F28" s="19">
+        <v>5727.1704</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="16">
+        <v>5681.0560999999998</v>
+      </c>
+      <c r="F29" s="19">
+        <v>5679.4859999999999</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Trained two more trials for 5K
</commit_message>
<xml_diff>
--- a/model_testing/shortjokesclean/shortjokesclean.xlsx
+++ b/model_testing/shortjokesclean/shortjokesclean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malik Shalash\Documents\Development\School\CECS-696\gpt-2-joker-bot\model_testing\shortjokesclean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7DD1C6-ADBF-41BA-AB61-5BF404B3C0BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56513FCD-A8EB-4274-9C93-F1BBAC70BF05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>Batch Size</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Loss 8</t>
+  </si>
+  <si>
+    <t>Top-K</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -392,6 +395,15 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -402,7 +414,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -432,6 +444,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -718,7 +732,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,12 +788,12 @@
         <v>14</v>
       </c>
       <c r="E3" s="1">
-        <f>3038.63/60</f>
-        <v>50.643833333333333</v>
+        <f>3070.1/60</f>
+        <v>51.168333333333329</v>
       </c>
       <c r="F3" s="1">
-        <f>3030.56/60</f>
-        <v>50.509333333333331</v>
+        <f>3078.88/60</f>
+        <v>51.314666666666668</v>
       </c>
       <c r="G3" s="1">
         <f>3026.82/60</f>
@@ -801,24 +815,18 @@
       <c r="B4" s="7">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5671.29</v>
-      </c>
-      <c r="F4" s="2">
-        <v>5679.85</v>
-      </c>
-      <c r="G4" s="2">
-        <v>5689.75</v>
-      </c>
-      <c r="H4" s="2">
-        <v>5689.02</v>
-      </c>
-      <c r="I4" s="2">
-        <v>5689.71</v>
-      </c>
+      <c r="D4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="23">
+        <v>7240.85</v>
+      </c>
+      <c r="F4" s="23">
+        <v>7260.51</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -827,14 +835,18 @@
       <c r="B5" s="6">
         <v>5000</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="D5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="23">
+        <v>6812.4</v>
+      </c>
+      <c r="F5" s="23">
+        <v>6809.6660000000002</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -843,6 +855,18 @@
       <c r="B6" s="6">
         <v>5000</v>
       </c>
+      <c r="D6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="23">
+        <v>6198.62</v>
+      </c>
+      <c r="F6" s="23">
+        <v>6195.66</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -851,6 +875,18 @@
       <c r="B7" s="6">
         <v>400</v>
       </c>
+      <c r="D7" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="23">
+        <v>6011.31</v>
+      </c>
+      <c r="F7" s="23">
+        <v>6009.18</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -859,6 +895,18 @@
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="D8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="23">
+        <v>5893.37</v>
+      </c>
+      <c r="F8" s="23">
+        <v>5883.9</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -867,6 +915,18 @@
       <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="D9" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="23">
+        <v>5820.57</v>
+      </c>
+      <c r="F9" s="23">
+        <v>5824.2</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -875,6 +935,66 @@
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="D10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="23">
+        <v>5758.31</v>
+      </c>
+      <c r="F10" s="23">
+        <v>5764.5219999999999</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="D11" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="23">
+        <v>5731.7</v>
+      </c>
+      <c r="F11" s="23">
+        <v>5715.0379999999996</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5672.17</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5682.73</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5689.75</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5689.02</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5689.71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1074,6 +1194,10 @@
       <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="24"/>
       <c r="D28" s="22" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Ran another 5K trial
</commit_message>
<xml_diff>
--- a/model_testing/shortjokesclean/shortjokesclean.xlsx
+++ b/model_testing/shortjokesclean/shortjokesclean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malik Shalash\Documents\Development\School\CECS-696\gpt-2-joker-bot\model_testing\shortjokesclean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56513FCD-A8EB-4274-9C93-F1BBAC70BF05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3094FA4B-5043-4A84-8A10-E09A4B4C1F0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,7 +732,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,8 +796,8 @@
         <v>51.314666666666668</v>
       </c>
       <c r="G3" s="1">
-        <f>3026.82/60</f>
-        <v>50.447000000000003</v>
+        <f>3052.63/60</f>
+        <v>50.877166666666668</v>
       </c>
       <c r="H3" s="1">
         <f>3049.82/60</f>
@@ -824,7 +824,9 @@
       <c r="F4" s="23">
         <v>7260.51</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="23">
+        <v>7247.31</v>
+      </c>
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
     </row>
@@ -844,7 +846,9 @@
       <c r="F5" s="23">
         <v>6809.6660000000002</v>
       </c>
-      <c r="G5" s="23"/>
+      <c r="G5" s="23">
+        <v>6808.2</v>
+      </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
     </row>
@@ -864,7 +868,9 @@
       <c r="F6" s="23">
         <v>6195.66</v>
       </c>
-      <c r="G6" s="23"/>
+      <c r="G6" s="23">
+        <v>6220.42</v>
+      </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
     </row>
@@ -884,7 +890,9 @@
       <c r="F7" s="23">
         <v>6009.18</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="23">
+        <v>6007.96</v>
+      </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
     </row>
@@ -904,7 +912,9 @@
       <c r="F8" s="23">
         <v>5883.9</v>
       </c>
-      <c r="G8" s="23"/>
+      <c r="G8" s="23">
+        <v>5893.0709999999999</v>
+      </c>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
     </row>
@@ -924,7 +934,9 @@
       <c r="F9" s="23">
         <v>5824.2</v>
       </c>
-      <c r="G9" s="23"/>
+      <c r="G9" s="23">
+        <v>5816.88</v>
+      </c>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
     </row>
@@ -944,7 +956,9 @@
       <c r="F10" s="23">
         <v>5764.5219999999999</v>
       </c>
-      <c r="G10" s="23"/>
+      <c r="G10" s="23">
+        <v>5760.1350000000002</v>
+      </c>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
     </row>
@@ -962,7 +976,9 @@
       <c r="F11" s="23">
         <v>5715.0379999999996</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="23">
+        <v>5722.85</v>
+      </c>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
     </row>
@@ -977,7 +993,7 @@
         <v>5682.73</v>
       </c>
       <c r="G12" s="2">
-        <v>5689.75</v>
+        <v>5677.7563399999999</v>
       </c>
       <c r="H12" s="2">
         <v>5689.02</v>

</xml_diff>

<commit_message>
Ran a 10K Trial
</commit_message>
<xml_diff>
--- a/model_testing/shortjokesclean/shortjokesclean.xlsx
+++ b/model_testing/shortjokesclean/shortjokesclean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malik Shalash\Documents\Development\School\CECS-696\gpt-2-joker-bot\model_testing\shortjokesclean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3094FA4B-5043-4A84-8A10-E09A4B4C1F0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CE07D7-0589-49C9-B56B-C6814B64886D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,12 +800,12 @@
         <v>50.877166666666668</v>
       </c>
       <c r="H3" s="1">
-        <f>3049.82/60</f>
-        <v>50.830333333333336</v>
+        <f>3164/60</f>
+        <v>52.733333333333334</v>
       </c>
       <c r="I3" s="1">
-        <f>3039.53/60</f>
-        <v>50.658833333333334</v>
+        <f>3075.63/60</f>
+        <v>51.2605</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -827,8 +827,12 @@
       <c r="G4" s="23">
         <v>7247.31</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
+      <c r="H4" s="23">
+        <v>7242.0590000000002</v>
+      </c>
+      <c r="I4" s="23">
+        <v>7240.92</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -849,8 +853,12 @@
       <c r="G5" s="23">
         <v>6808.2</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
+      <c r="H5" s="23">
+        <v>6823.4129999999996</v>
+      </c>
+      <c r="I5" s="23">
+        <v>6811.6580000000004</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -871,8 +879,12 @@
       <c r="G6" s="23">
         <v>6220.42</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
+      <c r="H6" s="23">
+        <v>6195.8760000000002</v>
+      </c>
+      <c r="I6" s="23">
+        <v>6188.82</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -893,8 +905,12 @@
       <c r="G7" s="23">
         <v>6007.96</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
+      <c r="H7" s="23">
+        <v>6005.3890000000001</v>
+      </c>
+      <c r="I7" s="23">
+        <v>6004.16</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -915,8 +931,12 @@
       <c r="G8" s="23">
         <v>5893.0709999999999</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
+      <c r="H8" s="23">
+        <v>5888.1289999999999</v>
+      </c>
+      <c r="I8" s="23">
+        <v>5899.2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -937,8 +957,12 @@
       <c r="G9" s="23">
         <v>5816.88</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
+      <c r="H9" s="23">
+        <v>5830.8779999999997</v>
+      </c>
+      <c r="I9" s="23">
+        <v>5824.96</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -959,8 +983,12 @@
       <c r="G10" s="23">
         <v>5760.1350000000002</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
+      <c r="H10" s="23">
+        <v>5778.79</v>
+      </c>
+      <c r="I10" s="23">
+        <v>5775.0259999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
@@ -979,8 +1007,12 @@
       <c r="G11" s="23">
         <v>5722.85</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
+      <c r="H11" s="23">
+        <v>5713.4859999999999</v>
+      </c>
+      <c r="I11" s="23">
+        <v>5716.5450000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="10" t="s">
@@ -996,10 +1028,10 @@
         <v>5677.7563399999999</v>
       </c>
       <c r="H12" s="2">
-        <v>5689.02</v>
+        <v>5678.3440000000001</v>
       </c>
       <c r="I12" s="2">
-        <v>5689.71</v>
+        <v>5679.7979999999998</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1060,13 +1092,20 @@
         <v>14</v>
       </c>
       <c r="E20" s="21">
-        <v>3068.42</v>
+        <f>3068.42/60</f>
+        <v>51.140333333333338</v>
       </c>
       <c r="F20" s="18">
-        <v>3052.0412999999999</v>
-      </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
+        <f>3052.0413/60</f>
+        <v>50.867354999999996</v>
+      </c>
+      <c r="G20" s="18">
+        <f>3142.41/60</f>
+        <v>52.3735</v>
+      </c>
+      <c r="H20" s="18">
+        <v>3076.92</v>
+      </c>
       <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1085,8 +1124,12 @@
       <c r="F21" s="19">
         <v>7240.6790000000001</v>
       </c>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="G21" s="19">
+        <v>7247.39</v>
+      </c>
+      <c r="H21" s="19">
+        <v>7247.76</v>
+      </c>
       <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1105,8 +1148,12 @@
       <c r="F22" s="19">
         <v>6808.009</v>
       </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="G22" s="19">
+        <v>6814.16</v>
+      </c>
+      <c r="H22" s="19">
+        <v>6810.9179999999997</v>
+      </c>
       <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1125,8 +1172,12 @@
       <c r="F23" s="19">
         <v>6191.0739999999996</v>
       </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="G23" s="19">
+        <v>6210.27</v>
+      </c>
+      <c r="H23" s="19">
+        <v>6212.24</v>
+      </c>
       <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1145,8 +1196,12 @@
       <c r="F24" s="19">
         <v>5998.9139999999998</v>
       </c>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="G24" s="19">
+        <v>5997.49</v>
+      </c>
+      <c r="H24" s="19">
+        <v>5999.83</v>
+      </c>
       <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1165,8 +1220,12 @@
       <c r="F25" s="19">
         <v>5897.4059999999999</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="G25" s="19">
+        <v>5894.78</v>
+      </c>
+      <c r="H25" s="19">
+        <v>5884.15</v>
+      </c>
       <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1185,8 +1244,12 @@
       <c r="F26" s="19">
         <v>5826.5320000000002</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="G26" s="19">
+        <v>5825.98</v>
+      </c>
+      <c r="H26" s="19">
+        <v>5816.6270000000004</v>
+      </c>
       <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,8 +1268,12 @@
       <c r="F27" s="19">
         <v>5770.317</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="G27" s="19">
+        <v>5760.25</v>
+      </c>
+      <c r="H27" s="19">
+        <v>5760.44</v>
+      </c>
       <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1223,8 +1290,12 @@
       <c r="F28" s="19">
         <v>5727.1704</v>
       </c>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="G28" s="19">
+        <v>5718.71</v>
+      </c>
+      <c r="H28" s="19">
+        <v>5721.83</v>
+      </c>
       <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1237,8 +1308,12 @@
       <c r="F29" s="19">
         <v>5679.4859999999999</v>
       </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="G29" s="19">
+        <v>5674.14</v>
+      </c>
+      <c r="H29" s="19">
+        <v>5690.62</v>
+      </c>
       <c r="I29" s="19"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ran last 10K trial
</commit_message>
<xml_diff>
--- a/model_testing/shortjokesclean/shortjokesclean.xlsx
+++ b/model_testing/shortjokesclean/shortjokesclean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malik Shalash\Documents\Development\School\CECS-696\gpt-2-joker-bot\model_testing\shortjokesclean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CE07D7-0589-49C9-B56B-C6814B64886D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7D6F92-DA3E-42F0-BE85-FD667285DAEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,9 +1104,13 @@
         <v>52.3735</v>
       </c>
       <c r="H20" s="18">
-        <v>3076.92</v>
-      </c>
-      <c r="I20" s="18"/>
+        <f>3076.92/60</f>
+        <v>51.282000000000004</v>
+      </c>
+      <c r="I20" s="18">
+        <f>3099.55/60</f>
+        <v>51.659166666666671</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -1130,7 +1134,9 @@
       <c r="H21" s="19">
         <v>7247.76</v>
       </c>
-      <c r="I21" s="19"/>
+      <c r="I21" s="19">
+        <v>7249.76</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1154,7 +1160,9 @@
       <c r="H22" s="19">
         <v>6810.9179999999997</v>
       </c>
-      <c r="I22" s="19"/>
+      <c r="I22" s="19">
+        <v>6812.75</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1178,7 +1186,9 @@
       <c r="H23" s="19">
         <v>6212.24</v>
       </c>
-      <c r="I23" s="19"/>
+      <c r="I23" s="19">
+        <v>6209.46</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1202,7 +1212,9 @@
       <c r="H24" s="19">
         <v>5999.83</v>
       </c>
-      <c r="I24" s="19"/>
+      <c r="I24" s="19">
+        <v>5994.1</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -1226,7 +1238,9 @@
       <c r="H25" s="19">
         <v>5884.15</v>
       </c>
-      <c r="I25" s="19"/>
+      <c r="I25" s="19">
+        <v>5885.34</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1250,7 +1264,9 @@
       <c r="H26" s="19">
         <v>5816.6270000000004</v>
       </c>
-      <c r="I26" s="19"/>
+      <c r="I26" s="19">
+        <v>5815.4</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -1274,7 +1290,9 @@
       <c r="H27" s="19">
         <v>5760.44</v>
       </c>
-      <c r="I27" s="19"/>
+      <c r="I27" s="19">
+        <v>5774.0110000000004</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -1296,7 +1314,9 @@
       <c r="H28" s="19">
         <v>5721.83</v>
       </c>
-      <c r="I28" s="19"/>
+      <c r="I28" s="19">
+        <v>5720.67</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D29" s="10" t="s">
@@ -1314,7 +1334,9 @@
       <c r="H29" s="19">
         <v>5690.62</v>
       </c>
-      <c r="I29" s="19"/>
+      <c r="I29" s="19">
+        <v>5682.38</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D30" s="10" t="s">

</xml_diff>

<commit_message>
Updated results sheet for 2E trials
</commit_message>
<xml_diff>
--- a/model_testing/shortjokesclean/shortjokesclean.xlsx
+++ b/model_testing/shortjokesclean/shortjokesclean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malik Shalash\Documents\Development\School\CECS-696\gpt-2-joker-bot\model_testing\shortjokesclean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055D72A0-8A3E-4773-95D6-BFAEBA3A63DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044EF034-ED7C-4E89-8A2F-7CE3D651A832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="37">
   <si>
     <t>Batch Size</t>
   </si>
@@ -125,6 +125,27 @@
   </si>
   <si>
     <t>Hyperparams (2E)</t>
+  </si>
+  <si>
+    <t>1(E2)</t>
+  </si>
+  <si>
+    <t>2(E2)</t>
+  </si>
+  <si>
+    <t>3(E3)</t>
+  </si>
+  <si>
+    <t>4(E4)</t>
+  </si>
+  <si>
+    <t>Epoch Min Loss</t>
+  </si>
+  <si>
+    <t>Train Time (Min)</t>
+  </si>
+  <si>
+    <t>NK</t>
   </si>
 </sst>
 </file>
@@ -191,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -530,6 +551,17 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -540,7 +572,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
@@ -563,37 +595,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1"/>
@@ -602,37 +610,90 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -920,7 +981,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,37 +992,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3">
@@ -983,13 +1044,13 @@
       <c r="H3" s="7">
         <v>4</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="24">
         <v>5</v>
       </c>
-      <c r="J3" s="24"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3">
@@ -1019,10 +1080,10 @@
         <f>3075.63/60</f>
         <v>51.2605</v>
       </c>
-      <c r="J4" s="24"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4">
@@ -1044,13 +1105,13 @@
       <c r="H5" s="14">
         <v>7242.0590000000002</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="22">
         <v>7240.92</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3">
@@ -1072,13 +1133,13 @@
       <c r="H6" s="14">
         <v>6823.4129999999996</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="22">
         <v>6811.6580000000004</v>
       </c>
-      <c r="J6" s="24"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3">
@@ -1100,13 +1161,13 @@
       <c r="H7" s="14">
         <v>6195.8760000000002</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="22">
         <v>6188.82</v>
       </c>
-      <c r="J7" s="24"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3">
@@ -1128,13 +1189,13 @@
       <c r="H8" s="14">
         <v>6005.3890000000001</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="22">
         <v>6004.16</v>
       </c>
-      <c r="J8" s="24"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1156,13 +1217,13 @@
       <c r="H9" s="14">
         <v>5888.1289999999999</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="22">
         <v>5899.2</v>
       </c>
-      <c r="J9" s="24"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1184,13 +1245,13 @@
       <c r="H10" s="14">
         <v>5830.8779999999997</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="22">
         <v>5824.96</v>
       </c>
-      <c r="J10" s="24"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1212,10 +1273,10 @@
       <c r="H11" s="14">
         <v>5778.79</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="22">
         <v>5775.0259999999998</v>
       </c>
-      <c r="J11" s="24"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -1236,10 +1297,10 @@
       <c r="H12" s="14">
         <v>5713.4859999999999</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="22">
         <v>5716.5450000000001</v>
       </c>
-      <c r="J12" s="24"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
@@ -1263,59 +1324,65 @@
       <c r="I13" s="8">
         <v>5679.7979999999998</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="24"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="42"/>
+      <c r="H14" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="24"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1333,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,43 +1411,43 @@
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
     <col min="14" max="14" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3">
@@ -1402,13 +1469,13 @@
       <c r="H3" s="7">
         <v>4</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="24">
         <v>5</v>
       </c>
-      <c r="J3" s="24"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3">
@@ -1416,7 +1483,7 @@
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="6" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1">
         <f>3070.1/60</f>
@@ -1438,10 +1505,10 @@
         <f>3075.63/60</f>
         <v>51.2605</v>
       </c>
-      <c r="J4" s="24"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4">
@@ -1463,13 +1530,13 @@
       <c r="H5" s="14">
         <v>7242.0590000000002</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="22">
         <v>7240.92</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3">
@@ -1491,13 +1558,13 @@
       <c r="H6" s="14">
         <v>6823.4129999999996</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="22">
         <v>6811.6580000000004</v>
       </c>
-      <c r="J6" s="24"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3">
@@ -1519,13 +1586,13 @@
       <c r="H7" s="14">
         <v>6195.8760000000002</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="22">
         <v>6188.82</v>
       </c>
-      <c r="J7" s="24"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3">
@@ -1547,13 +1614,13 @@
       <c r="H8" s="14">
         <v>6005.3890000000001</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="22">
         <v>6004.16</v>
       </c>
-      <c r="J8" s="24"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1575,13 +1642,13 @@
       <c r="H9" s="14">
         <v>5888.1289999999999</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="22">
         <v>5899.2</v>
       </c>
-      <c r="J9" s="24"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1603,13 +1670,13 @@
       <c r="H10" s="14">
         <v>5830.8779999999997</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="22">
         <v>5824.96</v>
       </c>
-      <c r="J10" s="24"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1631,10 +1698,10 @@
       <c r="H11" s="14">
         <v>5778.79</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="22">
         <v>5775.0259999999998</v>
       </c>
-      <c r="J11" s="24"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -1655,17 +1722,17 @@
       <c r="H12" s="14">
         <v>5713.4859999999999</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="22">
         <v>5716.5450000000001</v>
       </c>
-      <c r="J12" s="24"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E13" s="8">
         <v>5672.17</v>
@@ -1682,75 +1749,77 @@
       <c r="I13" s="8">
         <v>5679.7979999999998</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="24"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="42"/>
+      <c r="H14" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="24"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J18" s="24"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="D19" s="26" t="s">
+      <c r="B19" s="51"/>
+      <c r="D19" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="J19" s="24"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="50"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -1763,21 +1832,32 @@
       <c r="E20" s="7">
         <v>1</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="7">
         <v>2</v>
       </c>
-      <c r="G20" s="7">
+      <c r="H20" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="7">
         <v>3</v>
       </c>
-      <c r="H20" s="7">
+      <c r="J20" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="7">
         <v>4</v>
       </c>
-      <c r="I20" s="7">
+      <c r="L20" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="7">
         <v>5</v>
       </c>
-      <c r="J20" s="24"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -1785,205 +1865,318 @@
         <v>3</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="24"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E21" s="31"/>
+      <c r="F21" s="33">
+        <f>6512.6/60</f>
+        <v>108.54333333333334</v>
+      </c>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31">
+        <f>6373.24/60</f>
+        <v>106.22066666666666</v>
+      </c>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="4">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="24"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E22" s="11">
+        <v>7246.82</v>
+      </c>
+      <c r="F22" s="15">
+        <v>5638.66</v>
+      </c>
+      <c r="G22" s="11">
+        <v>7238.375</v>
+      </c>
+      <c r="H22" s="11">
+        <v>5645.6980000000003</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="3">
         <v>5000</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="24"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E23" s="11">
+        <v>6806.31</v>
+      </c>
+      <c r="F23" s="15">
+        <v>5607.835</v>
+      </c>
+      <c r="G23" s="11">
+        <v>6809.3789999999999</v>
+      </c>
+      <c r="H23" s="11">
+        <v>5603.3130000000001</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="3">
         <v>5000</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="24"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E24" s="11">
+        <v>6211.99</v>
+      </c>
+      <c r="F24" s="15">
+        <v>5596.9229999999998</v>
+      </c>
+      <c r="G24" s="11">
+        <v>6206.62</v>
+      </c>
+      <c r="H24" s="11">
+        <v>5563.81</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="3">
         <v>400</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="24"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E25" s="11">
+        <v>5999.8886000000002</v>
+      </c>
+      <c r="F25" s="58">
+        <v>5558.51</v>
+      </c>
+      <c r="G25" s="11">
+        <v>5990.65</v>
+      </c>
+      <c r="H25" s="11">
+        <v>5564.8690999999999</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="24"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E26" s="11">
+        <v>5885.5789999999997</v>
+      </c>
+      <c r="F26" s="58">
+        <v>5531.61</v>
+      </c>
+      <c r="G26" s="11">
+        <v>5899.1260000000002</v>
+      </c>
+      <c r="H26" s="11">
+        <v>5528</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="24"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E27" s="11">
+        <v>5815.01</v>
+      </c>
+      <c r="F27" s="58">
+        <v>5501.5659999999998</v>
+      </c>
+      <c r="G27" s="11">
+        <v>5820.2240000000002</v>
+      </c>
+      <c r="H27" s="11">
+        <v>5497.6779999999999</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="24"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D29" s="13" t="s">
+      <c r="E28" s="11">
+        <v>5768.7219999999998</v>
+      </c>
+      <c r="F28" s="58">
+        <v>5490.17</v>
+      </c>
+      <c r="G28" s="11">
+        <v>5757.98</v>
+      </c>
+      <c r="H28" s="11">
+        <v>5496.91</v>
+      </c>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D29" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="24"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E29" s="11">
+        <v>5723.73</v>
+      </c>
+      <c r="F29" s="58">
+        <v>5472.9290000000001</v>
+      </c>
+      <c r="G29" s="11">
+        <v>5728.95</v>
+      </c>
+      <c r="H29" s="11">
+        <v>5482.33</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="24"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="11">
+        <v>5674</v>
+      </c>
+      <c r="F30" s="11">
+        <v>5439.2740000000003</v>
+      </c>
+      <c r="G30" s="11">
+        <v>5688.79</v>
+      </c>
+      <c r="H30" s="11">
+        <v>5453</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D31" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="24"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D32" s="23" t="s">
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="24"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A19:B19"/>
+  <mergeCells count="18">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="E31:E32"/>
@@ -1997,6 +2190,11 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="E14:E15"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2008,7 +2206,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J17"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,37 +2216,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3">
@@ -2070,13 +2268,13 @@
       <c r="H3" s="7">
         <v>4</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="24">
         <v>5</v>
       </c>
-      <c r="J3" s="24"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3">
@@ -2106,10 +2304,10 @@
         <f>3075.63/60</f>
         <v>51.2605</v>
       </c>
-      <c r="J4" s="24"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4">
@@ -2131,13 +2329,13 @@
       <c r="H5" s="14">
         <v>7242.0590000000002</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="22">
         <v>7240.92</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3">
@@ -2159,13 +2357,13 @@
       <c r="H6" s="14">
         <v>6823.4129999999996</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="22">
         <v>6811.6580000000004</v>
       </c>
-      <c r="J6" s="24"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3">
@@ -2187,13 +2385,13 @@
       <c r="H7" s="14">
         <v>6195.8760000000002</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="22">
         <v>6188.82</v>
       </c>
-      <c r="J7" s="24"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3">
@@ -2215,13 +2413,13 @@
       <c r="H8" s="14">
         <v>6005.3890000000001</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="22">
         <v>6004.16</v>
       </c>
-      <c r="J8" s="24"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2243,13 +2441,13 @@
       <c r="H9" s="14">
         <v>5888.1289999999999</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="22">
         <v>5899.2</v>
       </c>
-      <c r="J9" s="24"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2271,13 +2469,13 @@
       <c r="H10" s="14">
         <v>5830.8779999999997</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="22">
         <v>5824.96</v>
       </c>
-      <c r="J10" s="24"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2299,10 +2497,10 @@
       <c r="H11" s="14">
         <v>5778.79</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="22">
         <v>5775.0259999999998</v>
       </c>
-      <c r="J11" s="24"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -2323,17 +2521,17 @@
       <c r="H12" s="14">
         <v>5713.4859999999999</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="22">
         <v>5716.5450000000001</v>
       </c>
-      <c r="J12" s="24"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E13" s="8">
         <v>5672.17</v>
@@ -2350,69 +2548,75 @@
       <c r="I13" s="8">
         <v>5679.7979999999998</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="24"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="42"/>
+      <c r="H14" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="24"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="27"/>
+      <c r="C18" s="20"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="D19" s="25" t="s">
+      <c r="B19" s="51"/>
+      <c r="D19" s="19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2677,7 +2881,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D30" s="6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E30" s="9">
         <v>5681.0560999999998</v>
@@ -2696,32 +2900,33 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="21"/>
+      <c r="E31" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" s="52" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="19"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
     <mergeCell ref="I31:I32"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:B2"/>
@@ -2730,6 +2935,11 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished third 3E trial
</commit_message>
<xml_diff>
--- a/model_testing/shortjokesclean/shortjokesclean.xlsx
+++ b/model_testing/shortjokesclean/shortjokesclean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malik Shalash\Documents\Development\School\CECS-696\gpt-2-joker-bot\model_testing\shortjokesclean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0442B2-BD79-4F7A-8FDA-D8A3D08EDCC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2130CDEA-5D33-4A0E-8464-FDF6AE140869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="930" windowWidth="10245" windowHeight="13845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="4" r:id="rId1"/>
@@ -673,30 +673,30 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
@@ -1425,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="C29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,14 +1833,14 @@
       <c r="J17" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="D19" s="52" t="s">
+      <c r="B19" s="55"/>
+      <c r="D19" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="52"/>
+      <c r="E19" s="53"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -2150,37 +2150,37 @@
       <c r="D31" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="57" t="s">
+      <c r="E31" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="56"/>
-      <c r="G31" s="57" t="s">
+      <c r="F31" s="51"/>
+      <c r="G31" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="H31" s="57" t="s">
+      <c r="H31" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="I31" s="57" t="s">
+      <c r="I31" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="56"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="55"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="58"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="55"/>
-      <c r="M32" s="55"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="54"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
@@ -2207,14 +2207,14 @@
       <c r="J34" s="18"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="D36" s="52" t="s">
+      <c r="B36" s="55"/>
+      <c r="D36" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="52"/>
+      <c r="E36" s="53"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -2278,7 +2278,10 @@
       </c>
       <c r="K38" s="31"/>
       <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
+      <c r="M38" s="31">
+        <f>9418/60</f>
+        <v>156.96666666666667</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -2308,9 +2311,15 @@
       <c r="J39" s="11">
         <v>5425.431640625</v>
       </c>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
+      <c r="K39" s="11">
+        <v>7240.2841796875</v>
+      </c>
+      <c r="L39" s="11">
+        <v>5629.93310546875</v>
+      </c>
+      <c r="M39" s="11">
+        <v>5413.2197265625</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -2340,9 +2349,15 @@
       <c r="J40" s="11">
         <v>5401.2001953125</v>
       </c>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
+      <c r="K40" s="11">
+        <v>6797.28076171875</v>
+      </c>
+      <c r="L40" s="11">
+        <v>5617.25537109375</v>
+      </c>
+      <c r="M40" s="11">
+        <v>5403.31005859375</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
@@ -2372,9 +2387,15 @@
       <c r="J41" s="11">
         <v>5391.3134765625</v>
       </c>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
+      <c r="K41" s="11">
+        <v>6199.29248046875</v>
+      </c>
+      <c r="L41" s="11">
+        <v>5586.822265625</v>
+      </c>
+      <c r="M41" s="11">
+        <v>5394.77587890625</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -2404,9 +2425,15 @@
       <c r="J42" s="11">
         <v>5363.7060546875</v>
       </c>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
+      <c r="K42" s="11">
+        <v>6010.1328125</v>
+      </c>
+      <c r="L42" s="11">
+        <v>5566.54296875</v>
+      </c>
+      <c r="M42" s="11">
+        <v>5379.45458984375</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -2436,9 +2463,15 @@
       <c r="J43" s="11">
         <v>5362.40478515625</v>
       </c>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
+      <c r="K43" s="11">
+        <v>5892.91845703125</v>
+      </c>
+      <c r="L43" s="11">
+        <v>5522.98388671875</v>
+      </c>
+      <c r="M43" s="11">
+        <v>5361.7548828125</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -2468,9 +2501,15 @@
       <c r="J44" s="11">
         <v>5353.34423828125</v>
       </c>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
+      <c r="K44" s="11">
+        <v>5823.51904296875</v>
+      </c>
+      <c r="L44" s="11">
+        <v>5507.3515625</v>
+      </c>
+      <c r="M44" s="11">
+        <v>5354.36181640625</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -2500,9 +2539,15 @@
       <c r="J45" s="11">
         <v>5331.888671875</v>
       </c>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
+      <c r="K45" s="11">
+        <v>5780.26123046875</v>
+      </c>
+      <c r="L45" s="11">
+        <v>5483.955078125</v>
+      </c>
+      <c r="M45" s="11">
+        <v>5328.583984375</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D46" s="32" t="s">
@@ -2526,9 +2571,15 @@
       <c r="J46" s="11">
         <v>5317.443359375</v>
       </c>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
+      <c r="K46" s="11">
+        <v>5720.65576171875</v>
+      </c>
+      <c r="L46" s="11">
+        <v>5457.41259765625</v>
+      </c>
+      <c r="M46" s="11">
+        <v>5315.52001953125</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D47" s="6" t="s">
@@ -2552,40 +2603,62 @@
       <c r="J47" s="11">
         <v>5310.08251953125</v>
       </c>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
+      <c r="K47" s="11">
+        <v>5683.27197265625</v>
+      </c>
+      <c r="L47" s="11">
+        <v>5456.05224609375</v>
+      </c>
+      <c r="M47" s="11">
+        <v>5310.7060546875</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D48" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E48" s="54"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="49"/>
-      <c r="J48" s="49"/>
-      <c r="K48" s="49"/>
-      <c r="L48" s="49"/>
-      <c r="M48" s="49"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
     </row>
     <row r="49" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="54"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="54"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
-      <c r="K49" s="50"/>
-      <c r="L49" s="50"/>
-      <c r="M49" s="50"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="L48:L49"/>
+    <mergeCell ref="K48:K49"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="E31:E32"/>
@@ -2599,22 +2672,6 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="M31:M32"/>
-    <mergeCell ref="L31:L32"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="K48:K49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3032,10 +3089,10 @@
       <c r="C18" s="20"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="53"/>
+      <c r="B19" s="55"/>
       <c r="D19" s="19" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Ran two 40K step trials
</commit_message>
<xml_diff>
--- a/model_testing/shortjokesclean/shortjokesclean.xlsx
+++ b/model_testing/shortjokesclean/shortjokesclean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malik Shalash\Documents\Development\School\CECS-696\gpt-2-joker-bot\model_testing\shortjokesclean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A358667F-2296-4A66-9BA2-0E91791763ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972CCB0A-87AB-48EA-8EEC-C3459F140F9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11310" yWindow="2910" windowWidth="10245" windowHeight="13845" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10110" yWindow="1905" windowWidth="10245" windowHeight="13845" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="42">
   <si>
     <t>Batch Size</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>Hyperparams (TS = 40K)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -575,7 +572,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
@@ -630,6 +627,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,47 +664,47 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1002,24 +1003,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="11"/>
       <c r="D2" s="25" t="s">
         <v>16</v>
@@ -1343,15 +1344,15 @@
       <c r="D14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="43" t="s">
+      <c r="E14" s="45"/>
+      <c r="F14" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="41"/>
-      <c r="H14" s="43" t="s">
+      <c r="G14" s="45"/>
+      <c r="H14" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="45" t="s">
+      <c r="I14" s="49" t="s">
         <v>34</v>
       </c>
       <c r="J14" s="16"/>
@@ -1363,11 +1364,11 @@
       <c r="D15" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="50"/>
       <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1427,24 +1428,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="11"/>
       <c r="D2" s="25" t="s">
         <v>16</v>
@@ -1768,15 +1769,15 @@
       <c r="D14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="43" t="s">
+      <c r="E14" s="45"/>
+      <c r="F14" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="41"/>
-      <c r="H14" s="43" t="s">
+      <c r="G14" s="45"/>
+      <c r="H14" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="45" t="s">
+      <c r="I14" s="49" t="s">
         <v>34</v>
       </c>
       <c r="J14" s="16"/>
@@ -1788,11 +1789,11 @@
       <c r="D15" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="50"/>
       <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1820,14 +1821,14 @@
       <c r="J17" s="16"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="D19" s="50" t="s">
+      <c r="B19" s="57"/>
+      <c r="D19" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="50"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -2137,37 +2138,37 @@
       <c r="D31" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F31" s="54"/>
-      <c r="G31" s="55" t="s">
+      <c r="F31" s="53"/>
+      <c r="G31" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="55" t="s">
+      <c r="H31" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I31" s="55" t="s">
+      <c r="I31" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="J31" s="54"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="56"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="53"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
@@ -2194,14 +2195,14 @@
       <c r="J34" s="16"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="D36" s="50" t="s">
+      <c r="B36" s="57"/>
+      <c r="D36" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="50"/>
+      <c r="E36" s="55"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -2604,38 +2605,54 @@
       <c r="D48" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E48" s="52"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="58" t="s">
+      <c r="E48" s="58"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="I48" s="57" t="s">
+      <c r="I48" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="J48" s="57" t="s">
+      <c r="J48" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="K48" s="47"/>
-      <c r="L48" s="47"/>
-      <c r="M48" s="47"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="62"/>
+      <c r="M48" s="62"/>
     </row>
     <row r="49" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="52"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="56"/>
-      <c r="J49" s="56"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="54"/>
+      <c r="L49" s="54"/>
+      <c r="M49" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="L48:L49"/>
+    <mergeCell ref="K48:K49"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="E31:E32"/>
@@ -2649,22 +2666,6 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="M31:M32"/>
-    <mergeCell ref="L31:L32"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="K48:K49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2675,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82B98F5-392D-4811-9916-8E485EB541A2}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,29 +2688,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="35"/>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="50"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
@@ -3042,20 +3043,20 @@
       <c r="D14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55" t="s">
+      <c r="F14" s="53"/>
+      <c r="G14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="55" t="s">
+      <c r="H14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="55" t="s">
+      <c r="I14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="54"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
@@ -3064,12 +3065,12 @@
       <c r="D15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="56"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="48"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="54"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
@@ -3099,14 +3100,14 @@
       <c r="C18" s="17"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="D19" s="50" t="s">
+      <c r="B19" s="57"/>
+      <c r="D19" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="50"/>
+      <c r="E19" s="55"/>
       <c r="F19" s="35"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
@@ -3162,7 +3163,10 @@
         <v>101.61928222166667</v>
       </c>
       <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
+      <c r="J21" s="28">
+        <f>6246.89/60</f>
+        <v>104.11483333333334</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3186,10 +3190,12 @@
       <c r="H22" s="10">
         <v>5642.6845703125</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" s="10"/>
+      <c r="I22" s="39">
+        <v>7252.98583984375</v>
+      </c>
+      <c r="J22" s="39">
+        <v>5637.2197265625</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -3213,8 +3219,12 @@
       <c r="H23" s="10">
         <v>5607.18798828125</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="I23" s="39">
+        <v>6803.0830078125</v>
+      </c>
+      <c r="J23" s="39">
+        <v>5613.5341796875</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -3238,8 +3248,12 @@
       <c r="H24" s="10">
         <v>5587.43115234375</v>
       </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="I24" s="39">
+        <v>6200.25</v>
+      </c>
+      <c r="J24" s="39">
+        <v>5585.0205078125</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -3263,8 +3277,12 @@
       <c r="H25" s="10">
         <v>5545.79150390625</v>
       </c>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
+      <c r="I25" s="39">
+        <v>6009.28857421875</v>
+      </c>
+      <c r="J25" s="39">
+        <v>5555.88232421875</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -3288,8 +3306,12 @@
       <c r="H26" s="10">
         <v>5534.1484375</v>
       </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+      <c r="I26" s="39">
+        <v>5895.3935546875</v>
+      </c>
+      <c r="J26" s="39">
+        <v>5535.62890625</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -3313,8 +3335,12 @@
       <c r="H27" s="10">
         <v>5506.9365234375</v>
       </c>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
+      <c r="I27" s="39">
+        <v>5817.16943359375</v>
+      </c>
+      <c r="J27" s="39">
+        <v>5509.9228515625</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -3338,8 +3364,12 @@
       <c r="H28" s="10">
         <v>5492.26611328125</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="I28" s="39">
+        <v>5754.40966796875</v>
+      </c>
+      <c r="J28" s="39">
+        <v>5483.87255859375</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D29" s="29" t="s">
@@ -3357,8 +3387,12 @@
       <c r="H29" s="10">
         <v>5462.03466796875</v>
       </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="I29" s="39">
+        <v>5723.5498046875</v>
+      </c>
+      <c r="J29" s="39">
+        <v>5464.93212890625</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D30" s="6" t="s">
@@ -3376,30 +3410,38 @@
       <c r="H30" s="10">
         <v>5452.06787109375</v>
       </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
+      <c r="I30" s="39">
+        <v>5688.49951171875</v>
+      </c>
+      <c r="J30" s="39">
+        <v>5448.8701171875</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D31" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="64"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="54"/>
+      <c r="E31" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="65"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="53"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="65"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="48"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="54"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
@@ -3426,15 +3468,15 @@
       <c r="J35" s="16"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="51"/>
+      <c r="B37" s="57"/>
       <c r="C37" s="35"/>
-      <c r="D37" s="50" t="s">
+      <c r="D37" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="50"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
       <c r="H37" s="35"/>
@@ -3482,10 +3524,16 @@
       <c r="D39" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="37">
+        <f>6195.80342609999/60</f>
+        <v>103.26339043499983</v>
+      </c>
       <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
+      <c r="H39" s="28">
+        <f>6199.2498843/60</f>
+        <v>103.32083140500001</v>
+      </c>
       <c r="I39" s="28"/>
       <c r="J39" s="28"/>
     </row>
@@ -3500,10 +3548,18 @@
       <c r="D40" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="28"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
+      <c r="E40" s="28">
+        <v>7250.69580078125</v>
+      </c>
+      <c r="F40" s="30">
+        <v>5631.525390625</v>
+      </c>
+      <c r="G40" s="39">
+        <v>7242.5712890625</v>
+      </c>
+      <c r="H40" s="39">
+        <v>5681.75146484375</v>
+      </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
     </row>
@@ -3518,10 +3574,18 @@
       <c r="D41" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
+      <c r="E41" s="39">
+        <v>6824.03466796875</v>
+      </c>
+      <c r="F41" s="38">
+        <v>5627.23193359375</v>
+      </c>
+      <c r="G41" s="39">
+        <v>6808.5537109375</v>
+      </c>
+      <c r="H41" s="39">
+        <v>5648.3115234375</v>
+      </c>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
     </row>
@@ -3536,10 +3600,18 @@
       <c r="D42" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
+      <c r="E42" s="39">
+        <v>6193.3447265625</v>
+      </c>
+      <c r="F42" s="38">
+        <v>5568.70751953125</v>
+      </c>
+      <c r="G42" s="39">
+        <v>6192.2099609375</v>
+      </c>
+      <c r="H42" s="39">
+        <v>5604.3173828125</v>
+      </c>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
@@ -3554,10 +3626,18 @@
       <c r="D43" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
+      <c r="E43" s="39">
+        <v>5989.95361328125</v>
+      </c>
+      <c r="F43" s="38">
+        <v>5556.40625</v>
+      </c>
+      <c r="G43" s="39">
+        <v>6011.7978515625</v>
+      </c>
+      <c r="H43" s="39">
+        <v>5582.75048828125</v>
+      </c>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
     </row>
@@ -3572,10 +3652,18 @@
       <c r="D44" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="10"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
+      <c r="E44" s="39">
+        <v>5893.5107421875</v>
+      </c>
+      <c r="F44" s="33">
+        <v>5530.314453125</v>
+      </c>
+      <c r="G44" s="39">
+        <v>5892.80078125</v>
+      </c>
+      <c r="H44" s="39">
+        <v>5560.90673828125</v>
+      </c>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
     </row>
@@ -3590,10 +3678,18 @@
       <c r="D45" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="10"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
+      <c r="E45" s="39">
+        <v>5822.6474609375</v>
+      </c>
+      <c r="F45" s="33">
+        <v>5512.14599609375</v>
+      </c>
+      <c r="G45" s="39">
+        <v>5830.47216796875</v>
+      </c>
+      <c r="H45" s="39">
+        <v>5530.97119140625</v>
+      </c>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
     </row>
@@ -3608,10 +3704,18 @@
       <c r="D46" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="10"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
+      <c r="E46" s="39">
+        <v>5771.412109375</v>
+      </c>
+      <c r="F46" s="33">
+        <v>5484.1953125</v>
+      </c>
+      <c r="G46" s="39">
+        <v>5759.51953125</v>
+      </c>
+      <c r="H46" s="39">
+        <v>5506.005859375</v>
+      </c>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
     </row>
@@ -3622,10 +3726,18 @@
       <c r="D47" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="10"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
+      <c r="E47" s="39">
+        <v>5715.740234375</v>
+      </c>
+      <c r="F47" s="33">
+        <v>5474.546875</v>
+      </c>
+      <c r="G47" s="39">
+        <v>5721.97509765625</v>
+      </c>
+      <c r="H47" s="39">
+        <v>5474.033203125</v>
+      </c>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
     </row>
@@ -3636,10 +3748,18 @@
       <c r="D48" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
+      <c r="E48" s="39">
+        <v>5683.671875</v>
+      </c>
+      <c r="F48" s="33">
+        <v>5457.43359375</v>
+      </c>
+      <c r="G48" s="39">
+        <v>5721.97509765625</v>
+      </c>
+      <c r="H48" s="39">
+        <v>5452.60009765625</v>
+      </c>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
     </row>
@@ -3650,12 +3770,12 @@
       <c r="D49" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="64"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="60"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="64"/>
-      <c r="J49" s="54"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="65"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="53"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="35"/>
@@ -3664,21 +3784,18 @@
       <c r="D50" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="65"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="65"/>
-      <c r="J50" s="48"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="68"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="J49:J50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="D19:E19"/>
@@ -3695,9 +3812,12 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="I49:I50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>